<commit_message>
Update Appendix A-Classwise Count detail.xlsx
</commit_message>
<xml_diff>
--- a/appendix/Appendix A-Classwise Count detail.xlsx
+++ b/appendix/Appendix A-Classwise Count detail.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Punit mam work 21 july 2021\draft paper 5 july 2022\final paper with figures 30 Sep 2022\Appendices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESKAPEE work 21 july 2021\draft paper 5 july 2022\final paper with figures 30 Sep 2022\Appendices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105790D-A1AD-473C-A9A7-E72AAD65B0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496193A9-1C54-4305-BE16-5A6DA9803C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15E92223-4AE0-4CDD-B0E8-A9057DC63605}"/>
   </bookViews>
   <sheets>
-    <sheet name="All class breakup" sheetId="1" r:id="rId1"/>
-    <sheet name="NonESKAPEE Bacteria" sheetId="3" r:id="rId2"/>
-    <sheet name=" Special NonESKAPEE bacteria" sheetId="4" r:id="rId3"/>
+    <sheet name="Names of Species" sheetId="5" r:id="rId1"/>
+    <sheet name="All class breakup" sheetId="1" r:id="rId2"/>
+    <sheet name="NonESKAPEE Bacteria" sheetId="3" r:id="rId3"/>
+    <sheet name=" Special NonESKAPEE bacteria" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_Hlk120479029" localSheetId="0">'Names of Species'!$C$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="179">
   <si>
     <t>Staphylococcus aureus</t>
   </si>
@@ -442,13 +446,145 @@
   </si>
   <si>
     <t>Count of samples under each of the 11 classes including 8 ESKAPEE and 3 Non-ESKAPEE</t>
+  </si>
+  <si>
+    <t>Specie Name</t>
+  </si>
+  <si>
+    <t>ESKAPEE bacteria Category</t>
+  </si>
+  <si>
+    <t>Non-ESKAPEE bacteria Category</t>
+  </si>
+  <si>
+    <t>Special non-ESKAPEE Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus faecium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus casseliflavus </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus hirae </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus mundtii </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus phage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterococcus faecalis </t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>Staphylococcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staphylococcus aureus </t>
+  </si>
+  <si>
+    <t>Staphylococcus_carnosus</t>
+  </si>
+  <si>
+    <t>Staphylococcus_pasteuri</t>
+  </si>
+  <si>
+    <t>Staphylococcus viyulinus</t>
+  </si>
+  <si>
+    <t>Klebsiella</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klebsiella pneumoniae </t>
+  </si>
+  <si>
+    <t>Acinetobacter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acinetobacter baumannii </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acinetobacter_ADP1_uid61597/   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acinetobacter_calcoaceticus_PHEA_2_uid83123/        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acinetobacter_oleivorans_DR1_uid50119/     </t>
+  </si>
+  <si>
+    <t>Acinetobacter_baylyi</t>
+  </si>
+  <si>
+    <t>Acinetobacter haemolyticus</t>
+  </si>
+  <si>
+    <t>Pseudomonas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas aeruginosa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas_ND6_uid167583/   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas_TKP_uid232248/    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas_VLB120_uid226717/   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudomonas_brassicacearum   </t>
+  </si>
+  <si>
+    <t>Pseudomonas_denitrificans</t>
+  </si>
+  <si>
+    <t>Enterobacter</t>
+  </si>
+  <si>
+    <t>Enterobacter amnigenus</t>
+  </si>
+  <si>
+    <t>Enterobacter kobei</t>
+  </si>
+  <si>
+    <t>Enterobacter hormaechei</t>
+  </si>
+  <si>
+    <t>Enterobacter taylorae</t>
+  </si>
+  <si>
+    <t>Enterobacter cloacae</t>
+  </si>
+  <si>
+    <t>Enterobacter aerogenes</t>
+  </si>
+  <si>
+    <t>E. Coli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escherichia coli </t>
+  </si>
+  <si>
+    <t>Names of Species considered in the Train/Test dataset under different categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These are the non-ESKAPEE categories considered in addition to those present at the link* </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +698,37 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -577,7 +744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -648,12 +815,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -776,6 +1037,57 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1098,10 +1410,486 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E37C63D6-1BC5-47BA-9484-975802E716DB}">
+  <dimension ref="C2:F48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="3:6" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="3:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C5" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="54"/>
+    </row>
+    <row r="7" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="54"/>
+    </row>
+    <row r="8" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="54"/>
+    </row>
+    <row r="9" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56" t="s">
+        <v>145</v>
+      </c>
+      <c r="F9" s="55"/>
+    </row>
+    <row r="10" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C22" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="F23" s="60" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="F24" s="60" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="53" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="61"/>
+    </row>
+    <row r="29" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="61"/>
+    </row>
+    <row r="30" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" s="61"/>
+    </row>
+    <row r="31" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="53" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="61"/>
+    </row>
+    <row r="32" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="61"/>
+    </row>
+    <row r="33" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="F33" s="61"/>
+    </row>
+    <row r="34" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" s="61"/>
+    </row>
+    <row r="35" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="61"/>
+    </row>
+    <row r="36" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="61"/>
+    </row>
+    <row r="37" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="61"/>
+    </row>
+    <row r="38" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="61"/>
+    </row>
+    <row r="39" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="61"/>
+    </row>
+    <row r="40" spans="3:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C40" s="54"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="61"/>
+    </row>
+    <row r="41" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" s="58"/>
+    </row>
+    <row r="42" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C42" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="52" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C43" s="54"/>
+      <c r="D43" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+    </row>
+    <row r="44" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C44" s="54"/>
+      <c r="D44" s="53" t="s">
+        <v>171</v>
+      </c>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+    </row>
+    <row r="45" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C45" s="54"/>
+      <c r="D45" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+    </row>
+    <row r="46" spans="3:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C46" s="54"/>
+      <c r="D46" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+    </row>
+    <row r="47" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C47" s="55"/>
+      <c r="D47" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+    </row>
+    <row r="48" spans="3:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C48" s="62" t="s">
+        <v>175</v>
+      </c>
+      <c r="D48" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E48" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" s="63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="E42:E47"/>
+    <mergeCell ref="F42:F47"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="C26:C41"/>
+    <mergeCell ref="D26:D41"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="F5:F9"/>
+    <mergeCell ref="C10:C19"/>
+    <mergeCell ref="D10:D19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A7C94D-D181-4BF4-BEBC-3E9E530FD078}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1368,12 +2156,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DF0E07-0302-4A9D-8864-B3999CD3A696}">
   <dimension ref="A1:AV714"/>
   <sheetViews>
     <sheetView zoomScale="104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5817,12 +6605,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BDB7499-C000-4659-A230-A6C5A41F597C}">
   <dimension ref="A1:AD52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5884,6 +6672,9 @@
       <c r="A3" s="27" t="s">
         <v>55</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="4" spans="1:30" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
@@ -5891,8 +6682,12 @@
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>95</v>
+      </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -7034,7 +7829,10 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B50">
     <sortCondition ref="A3:A50"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{14669861-CA3F-4E66-B398-79D372310971}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>